<commit_message>
Sparks 2.2.9 - finishing content
</commit_message>
<xml_diff>
--- a/sparks/img/U2/lab02/click-area-chart.xlsx
+++ b/sparks/img/U2/lab02/click-area-chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/bjc-r/sparks/img/U2/lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497BD218-D0F0-AB49-81F9-FBAB4DFDCE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA4BA2D-A261-104B-84D0-F3C8D34C91A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="2820" windowWidth="27640" windowHeight="16540" xr2:uid="{251B0E13-0F88-AE46-B47D-72CE204F2531}"/>
+    <workbookView xWindow="1160" yWindow="1460" windowWidth="27640" windowHeight="16540" xr2:uid="{251B0E13-0F88-AE46-B47D-72CE204F2531}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Click Area</t>
-  </si>
-  <si>
     <t>Mercury</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Minimum x</t>
+  </si>
+  <si>
+    <t>Click Area Name</t>
   </si>
 </sst>
 </file>
@@ -94,14 +94,14 @@
     </font>
     <font>
       <b/>
-      <sz val="24"/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Cavolini"/>
     </font>
@@ -157,16 +157,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,182 +486,185 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="A1:E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="5" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="4">
+        <v>-80</v>
+      </c>
+      <c r="C2" s="4">
+        <v>-240</v>
+      </c>
+      <c r="D2" s="4">
+        <v>180</v>
+      </c>
+      <c r="E2" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
+        <v>80</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-80</v>
+      </c>
+      <c r="D3" s="4">
+        <v>180</v>
+      </c>
+      <c r="E3" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B4" s="4">
+        <v>240</v>
+      </c>
+      <c r="C4" s="4">
+        <v>80</v>
+      </c>
+      <c r="D4" s="4">
+        <v>180</v>
+      </c>
+      <c r="E4" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
         <v>-80</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C5" s="4">
         <v>-240</v>
       </c>
-      <c r="D2" s="2">
-        <v>180</v>
-      </c>
-      <c r="E2" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="D5" s="4">
+        <v>40</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4">
         <v>80</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C6" s="4">
         <v>-80</v>
       </c>
-      <c r="D3" s="2">
-        <v>180</v>
-      </c>
-      <c r="E3" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="D6" s="4">
+        <v>40</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4">
         <v>240</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C7" s="4">
         <v>80</v>
       </c>
-      <c r="D4" s="2">
-        <v>180</v>
-      </c>
-      <c r="E4" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="D7" s="4">
+        <v>40</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
         <v>-80</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C8" s="4">
         <v>-240</v>
       </c>
-      <c r="D5" s="2">
-        <v>60</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="D8" s="4">
+        <v>-40</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
         <v>80</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C9" s="4">
         <v>-80</v>
       </c>
-      <c r="D6" s="2">
-        <v>60</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="D9" s="4">
+        <v>-40</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
         <v>240</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C10" s="4">
         <v>80</v>
       </c>
-      <c r="D7" s="2">
-        <v>60</v>
-      </c>
-      <c r="E7" s="2">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-80</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-240</v>
-      </c>
-      <c r="D8" s="2">
-        <v>-60</v>
-      </c>
-      <c r="E8" s="2">
-        <v>-180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>80</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-80</v>
-      </c>
-      <c r="D9" s="2">
-        <v>-60</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>240</v>
-      </c>
-      <c r="C10" s="2">
-        <v>80</v>
-      </c>
-      <c r="D10" s="2">
-        <v>-60</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="4">
+        <v>-40</v>
+      </c>
+      <c r="E10" s="4">
         <v>-180</v>
       </c>
     </row>

</xml_diff>